<commit_message>
new simulation results, now also for ilisu based on usgs data at mosul. added file main.Rmd where we will bring all of the pieces together.
</commit_message>
<xml_diff>
--- a/data/energy/energy_main.xlsx
+++ b/data/energy/energy_main.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/ETH/code/cciwr/data/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EEEED2-3F5F-E74C-AC27-88018B038711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8411D1C1-35F1-814B-87B4-42B29A5ABAF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3660" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Electricity consumption" sheetId="3" r:id="rId1"/>
-    <sheet name="Ilisu electricity generation" sheetId="6" r:id="rId2"/>
-    <sheet name="Electricity imports vs. exports" sheetId="1" r:id="rId3"/>
-    <sheet name="Renewable share in final energy" sheetId="4" r:id="rId4"/>
-    <sheet name="Renewable share in power produc" sheetId="5" r:id="rId5"/>
+    <sheet name="Ilisu electricity generation" sheetId="6" r:id="rId1"/>
+    <sheet name="Electricity demand (monthly) " sheetId="7" r:id="rId2"/>
+    <sheet name="Electricity consumption" sheetId="3" r:id="rId3"/>
+    <sheet name="Electricity imports vs. exports" sheetId="1" r:id="rId4"/>
+    <sheet name="Renewable share in final energy" sheetId="4" r:id="rId5"/>
+    <sheet name="Renewable share in power produc" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Source: IEA World Energy Balances 2019 https://www.iea.org/subscribe-to-data-services/world-energy-balances-and-statistics</t>
   </si>
@@ -163,6 +164,51 @@
   </si>
   <si>
     <t>TWh</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>Monthly electricity demand for Turkey</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/content/pdf/10.1007/s00521-017-3183-5.pdf</t>
   </si>
 </sst>
 </file>
@@ -312,13 +358,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -498,6 +546,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -615,7 +669,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -658,14 +712,17 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -699,6 +756,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2258,11 +2316,2398 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ED8B55-971D-A44A-BE5B-A8B57732300D}">
+  <dimension ref="A1:F86"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <f>E3/1000</f>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <v>3844</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1990</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1991</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1992</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1993</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1994</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1995</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1996</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1997</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1998</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1999</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2">
+        <v>11</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2001</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2002</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2003</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="2">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2004</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2005</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2">
+        <v>17</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2006</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2007</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2">
+        <v>19</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2008</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2">
+        <v>20</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2009</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2">
+        <v>21</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2010</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="2">
+        <v>22</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2011</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="2">
+        <v>23</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2012</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2">
+        <v>24</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2013</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="2">
+        <v>25</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="2">
+        <v>26</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2015</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="2">
+        <v>27</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2016</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="2">
+        <v>28</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="2">
+        <v>29</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="2">
+        <v>30</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="2">
+        <v>31</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2">
+        <v>32</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" ref="C37:C68" si="0">$B$3</f>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="2">
+        <v>33</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C38" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" ref="D38:D69" si="1">$B$3</f>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="2">
+        <v>34</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" ref="E39:E86" si="2">$B$3</f>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="2">
+        <v>35</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="2">
+        <v>36</v>
+      </c>
+      <c r="B41" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="2">
+        <v>37</v>
+      </c>
+      <c r="B42" s="2">
+        <v>2026</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="2">
+        <v>38</v>
+      </c>
+      <c r="B43" s="2">
+        <v>2027</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="2">
+        <v>39</v>
+      </c>
+      <c r="B44" s="2">
+        <v>2028</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="2">
+        <v>40</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2029</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="2">
+        <v>41</v>
+      </c>
+      <c r="B46" s="2">
+        <v>2030</v>
+      </c>
+      <c r="C46" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="2">
+        <v>42</v>
+      </c>
+      <c r="B47" s="2">
+        <v>2031</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="2">
+        <v>43</v>
+      </c>
+      <c r="B48" s="2">
+        <v>2032</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="2">
+        <v>44</v>
+      </c>
+      <c r="B49" s="2">
+        <v>2033</v>
+      </c>
+      <c r="C49" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E49" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="2">
+        <v>45</v>
+      </c>
+      <c r="B50" s="2">
+        <v>2034</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="2">
+        <v>46</v>
+      </c>
+      <c r="B51" s="2">
+        <v>2035</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E51" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="2">
+        <v>47</v>
+      </c>
+      <c r="B52" s="2">
+        <v>2036</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E52" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="2">
+        <v>48</v>
+      </c>
+      <c r="B53" s="2">
+        <v>2037</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="2">
+        <v>49</v>
+      </c>
+      <c r="B54" s="2">
+        <v>2038</v>
+      </c>
+      <c r="C54" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E54" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2">
+        <v>50</v>
+      </c>
+      <c r="B55" s="2">
+        <v>2039</v>
+      </c>
+      <c r="C55" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E55" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="2">
+        <v>51</v>
+      </c>
+      <c r="B56" s="2">
+        <v>2040</v>
+      </c>
+      <c r="C56" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E56" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="2">
+        <v>52</v>
+      </c>
+      <c r="B57" s="2">
+        <v>2041</v>
+      </c>
+      <c r="C57" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E57" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="2">
+        <v>53</v>
+      </c>
+      <c r="B58" s="2">
+        <v>2042</v>
+      </c>
+      <c r="C58" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D58" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E58" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="2">
+        <v>54</v>
+      </c>
+      <c r="B59" s="2">
+        <v>2043</v>
+      </c>
+      <c r="C59" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D59" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E59" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2">
+        <v>55</v>
+      </c>
+      <c r="B60" s="2">
+        <v>2044</v>
+      </c>
+      <c r="C60" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D60" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E60" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="2">
+        <v>56</v>
+      </c>
+      <c r="B61" s="2">
+        <v>2045</v>
+      </c>
+      <c r="C61" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D61" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E61" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2">
+        <v>57</v>
+      </c>
+      <c r="B62" s="2">
+        <v>2046</v>
+      </c>
+      <c r="C62" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D62" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E62" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2">
+        <v>58</v>
+      </c>
+      <c r="B63" s="2">
+        <v>2047</v>
+      </c>
+      <c r="C63" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D63" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E63" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="2">
+        <v>59</v>
+      </c>
+      <c r="B64" s="2">
+        <v>2048</v>
+      </c>
+      <c r="C64" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D64" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E64" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="2">
+        <v>60</v>
+      </c>
+      <c r="B65" s="2">
+        <v>2049</v>
+      </c>
+      <c r="C65" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D65" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E65" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="2">
+        <v>61</v>
+      </c>
+      <c r="B66" s="2">
+        <v>2050</v>
+      </c>
+      <c r="C66" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D66" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E66" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="2">
+        <v>62</v>
+      </c>
+      <c r="B67" s="2">
+        <v>2051</v>
+      </c>
+      <c r="C67" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D67" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E67" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="2">
+        <v>63</v>
+      </c>
+      <c r="B68" s="2">
+        <v>2052</v>
+      </c>
+      <c r="C68" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D68" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="2">
+        <v>64</v>
+      </c>
+      <c r="B69" s="2">
+        <v>2053</v>
+      </c>
+      <c r="C69" s="3">
+        <f t="shared" ref="C69:C86" si="3">$B$3</f>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D69" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E69" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="2">
+        <v>65</v>
+      </c>
+      <c r="B70" s="2">
+        <v>2054</v>
+      </c>
+      <c r="C70" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D70" s="3">
+        <f t="shared" ref="D70:D86" si="4">$B$3</f>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E70" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="2">
+        <v>66</v>
+      </c>
+      <c r="B71" s="2">
+        <v>2055</v>
+      </c>
+      <c r="C71" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D71" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E71" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="2">
+        <v>67</v>
+      </c>
+      <c r="B72" s="2">
+        <v>2056</v>
+      </c>
+      <c r="C72" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D72" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E72" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="2">
+        <v>68</v>
+      </c>
+      <c r="B73" s="2">
+        <v>2057</v>
+      </c>
+      <c r="C73" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D73" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E73" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="2">
+        <v>69</v>
+      </c>
+      <c r="B74" s="2">
+        <v>2058</v>
+      </c>
+      <c r="C74" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D74" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E74" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="2">
+        <v>70</v>
+      </c>
+      <c r="B75" s="2">
+        <v>2059</v>
+      </c>
+      <c r="C75" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D75" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E75" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="2">
+        <v>71</v>
+      </c>
+      <c r="B76" s="2">
+        <v>2060</v>
+      </c>
+      <c r="C76" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D76" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E76" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="2">
+        <v>72</v>
+      </c>
+      <c r="B77" s="2">
+        <v>2061</v>
+      </c>
+      <c r="C77" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D77" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E77" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="2">
+        <v>73</v>
+      </c>
+      <c r="B78" s="2">
+        <v>2062</v>
+      </c>
+      <c r="C78" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D78" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E78" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="2">
+        <v>74</v>
+      </c>
+      <c r="B79" s="2">
+        <v>2063</v>
+      </c>
+      <c r="C79" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D79" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E79" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="2">
+        <v>75</v>
+      </c>
+      <c r="B80" s="2">
+        <v>2064</v>
+      </c>
+      <c r="C80" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D80" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E80" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="2">
+        <v>76</v>
+      </c>
+      <c r="B81" s="2">
+        <v>2065</v>
+      </c>
+      <c r="C81" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D81" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E81" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="2">
+        <v>77</v>
+      </c>
+      <c r="B82" s="2">
+        <v>2066</v>
+      </c>
+      <c r="C82" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D82" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E82" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="2">
+        <v>78</v>
+      </c>
+      <c r="B83" s="2">
+        <v>2067</v>
+      </c>
+      <c r="C83" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D83" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E83" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="2">
+        <v>79</v>
+      </c>
+      <c r="B84" s="2">
+        <v>2068</v>
+      </c>
+      <c r="C84" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D84" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E84" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="2">
+        <v>80</v>
+      </c>
+      <c r="B85" s="2">
+        <v>2069</v>
+      </c>
+      <c r="C85" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D85" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E85" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="2">
+        <v>81</v>
+      </c>
+      <c r="B86" s="2">
+        <v>2070</v>
+      </c>
+      <c r="C86" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="D86" s="3">
+        <f t="shared" si="4"/>
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="E86" s="3">
+        <f t="shared" si="2"/>
+        <v>3.8439999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66409602-E0A5-AC48-B80A-4279EA23F232}">
+  <dimension ref="A1:R17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30:G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2002</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2003</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2004</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2005</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2006</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2007</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2008</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2009</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2010</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2011</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2012</v>
+      </c>
+      <c r="M5" s="2">
+        <v>2013</v>
+      </c>
+      <c r="N5" s="2">
+        <v>2014</v>
+      </c>
+      <c r="O5" s="4">
+        <v>2015</v>
+      </c>
+      <c r="P5" s="4">
+        <v>2016</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>2017</v>
+      </c>
+      <c r="R5" s="4">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2">
+        <v>11964</v>
+      </c>
+      <c r="C6" s="2">
+        <v>12386</v>
+      </c>
+      <c r="D6" s="2">
+        <v>12942</v>
+      </c>
+      <c r="E6" s="2">
+        <v>13212</v>
+      </c>
+      <c r="F6" s="2">
+        <v>14172</v>
+      </c>
+      <c r="G6" s="2">
+        <v>15686</v>
+      </c>
+      <c r="H6" s="2">
+        <v>17948</v>
+      </c>
+      <c r="I6" s="2">
+        <v>16851</v>
+      </c>
+      <c r="J6" s="2">
+        <v>17422</v>
+      </c>
+      <c r="K6" s="2">
+        <v>19724</v>
+      </c>
+      <c r="L6" s="2">
+        <v>21406</v>
+      </c>
+      <c r="M6" s="2">
+        <v>21275</v>
+      </c>
+      <c r="N6" s="2">
+        <v>21904</v>
+      </c>
+      <c r="O6" s="4">
+        <v>22338</v>
+      </c>
+      <c r="P6" s="4">
+        <v>22518</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>22653</v>
+      </c>
+      <c r="R6" s="4">
+        <v>22753</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2">
+        <v>9951</v>
+      </c>
+      <c r="C7" s="2">
+        <v>10859</v>
+      </c>
+      <c r="D7" s="2">
+        <v>11508</v>
+      </c>
+      <c r="E7" s="2">
+        <v>12524</v>
+      </c>
+      <c r="F7" s="2">
+        <v>13540</v>
+      </c>
+      <c r="G7" s="2">
+        <v>14548</v>
+      </c>
+      <c r="H7" s="2">
+        <v>16504</v>
+      </c>
+      <c r="I7" s="2">
+        <v>15010</v>
+      </c>
+      <c r="J7" s="2">
+        <v>15745</v>
+      </c>
+      <c r="K7" s="2">
+        <v>17790</v>
+      </c>
+      <c r="L7" s="2">
+        <v>19995</v>
+      </c>
+      <c r="M7" s="2">
+        <v>18842</v>
+      </c>
+      <c r="N7" s="2">
+        <v>19674</v>
+      </c>
+      <c r="O7" s="4">
+        <v>20587</v>
+      </c>
+      <c r="P7" s="4">
+        <v>20756</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>20883</v>
+      </c>
+      <c r="R7" s="4">
+        <v>20977</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2">
+        <v>11215</v>
+      </c>
+      <c r="C8" s="2">
+        <v>12391</v>
+      </c>
+      <c r="D8" s="2">
+        <v>12539</v>
+      </c>
+      <c r="E8" s="2">
+        <v>13466</v>
+      </c>
+      <c r="F8" s="2">
+        <v>14471</v>
+      </c>
+      <c r="G8" s="2">
+        <v>15623</v>
+      </c>
+      <c r="H8" s="2">
+        <v>16245</v>
+      </c>
+      <c r="I8" s="2">
+        <v>15984</v>
+      </c>
+      <c r="J8" s="2">
+        <v>17079</v>
+      </c>
+      <c r="K8" s="2">
+        <v>19278</v>
+      </c>
+      <c r="L8" s="2">
+        <v>20758</v>
+      </c>
+      <c r="M8" s="2">
+        <v>20464</v>
+      </c>
+      <c r="N8" s="2">
+        <v>20942</v>
+      </c>
+      <c r="O8" s="4">
+        <v>21392</v>
+      </c>
+      <c r="P8" s="4">
+        <v>21556</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>21679</v>
+      </c>
+      <c r="R8" s="4">
+        <v>21770</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10606</v>
+      </c>
+      <c r="C9" s="2">
+        <v>11045</v>
+      </c>
+      <c r="D9" s="2">
+        <v>11782</v>
+      </c>
+      <c r="E9" s="2">
+        <v>12534</v>
+      </c>
+      <c r="F9" s="2">
+        <v>13278</v>
+      </c>
+      <c r="G9" s="2">
+        <v>14786</v>
+      </c>
+      <c r="H9" s="2">
+        <v>15652</v>
+      </c>
+      <c r="I9" s="2">
+        <v>14849</v>
+      </c>
+      <c r="J9" s="2">
+        <v>16314</v>
+      </c>
+      <c r="K9" s="2">
+        <v>17923</v>
+      </c>
+      <c r="L9" s="2">
+        <v>18255</v>
+      </c>
+      <c r="M9" s="2">
+        <v>19139</v>
+      </c>
+      <c r="N9" s="2">
+        <v>20267</v>
+      </c>
+      <c r="O9" s="4">
+        <v>19714</v>
+      </c>
+      <c r="P9" s="4">
+        <v>19862</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>19973</v>
+      </c>
+      <c r="R9" s="4">
+        <v>20055</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2">
+        <v>10386</v>
+      </c>
+      <c r="C10" s="2">
+        <v>10918</v>
+      </c>
+      <c r="D10" s="2">
+        <v>11822</v>
+      </c>
+      <c r="E10" s="2">
+        <v>12760</v>
+      </c>
+      <c r="F10" s="2">
+        <v>13876</v>
+      </c>
+      <c r="G10" s="2">
+        <v>15113</v>
+      </c>
+      <c r="H10" s="2">
+        <v>16284</v>
+      </c>
+      <c r="I10" s="2">
+        <v>15298</v>
+      </c>
+      <c r="J10" s="2">
+        <v>16712</v>
+      </c>
+      <c r="K10" s="2">
+        <v>17686</v>
+      </c>
+      <c r="L10" s="2">
+        <v>18954</v>
+      </c>
+      <c r="M10" s="2">
+        <v>19512</v>
+      </c>
+      <c r="N10" s="2">
+        <v>20424</v>
+      </c>
+      <c r="O10" s="4">
+        <v>20253</v>
+      </c>
+      <c r="P10" s="4">
+        <v>20409</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>20525</v>
+      </c>
+      <c r="R10" s="4">
+        <v>20611</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10435</v>
+      </c>
+      <c r="C11" s="2">
+        <v>11085</v>
+      </c>
+      <c r="D11" s="2">
+        <v>11926</v>
+      </c>
+      <c r="E11" s="2">
+        <v>12603</v>
+      </c>
+      <c r="F11" s="2">
+        <v>14336</v>
+      </c>
+      <c r="G11" s="2">
+        <v>15560</v>
+      </c>
+      <c r="H11" s="2">
+        <v>16527</v>
+      </c>
+      <c r="I11" s="2">
+        <v>15900</v>
+      </c>
+      <c r="J11" s="2">
+        <v>17143</v>
+      </c>
+      <c r="K11" s="2">
+        <v>18003</v>
+      </c>
+      <c r="L11" s="2">
+        <v>20101</v>
+      </c>
+      <c r="M11" s="2">
+        <v>20133</v>
+      </c>
+      <c r="N11" s="2">
+        <v>20645</v>
+      </c>
+      <c r="O11" s="4">
+        <v>21139</v>
+      </c>
+      <c r="P11" s="4">
+        <v>21310</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>21437</v>
+      </c>
+      <c r="R11" s="4">
+        <v>21531</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11729</v>
+      </c>
+      <c r="C12" s="2">
+        <v>12415</v>
+      </c>
+      <c r="D12" s="2">
+        <v>13243</v>
+      </c>
+      <c r="E12" s="2">
+        <v>14254</v>
+      </c>
+      <c r="F12" s="2">
+        <v>15453</v>
+      </c>
+      <c r="G12" s="2">
+        <v>17492</v>
+      </c>
+      <c r="H12" s="2">
+        <v>18309</v>
+      </c>
+      <c r="I12" s="2">
+        <v>17744</v>
+      </c>
+      <c r="J12" s="2">
+        <v>19428</v>
+      </c>
+      <c r="K12" s="2">
+        <v>21070</v>
+      </c>
+      <c r="L12" s="2">
+        <v>22880</v>
+      </c>
+      <c r="M12" s="2">
+        <v>22649</v>
+      </c>
+      <c r="N12" s="2">
+        <v>23233</v>
+      </c>
+      <c r="O12" s="4">
+        <v>24213</v>
+      </c>
+      <c r="P12" s="4">
+        <v>24417</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>24570</v>
+      </c>
+      <c r="R12" s="4">
+        <v>24684</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="2">
+        <v>11647</v>
+      </c>
+      <c r="C13" s="2">
+        <v>12561</v>
+      </c>
+      <c r="D13" s="2">
+        <v>13305</v>
+      </c>
+      <c r="E13" s="2">
+        <v>14694</v>
+      </c>
+      <c r="F13" s="2">
+        <v>16267</v>
+      </c>
+      <c r="G13" s="2">
+        <v>17580</v>
+      </c>
+      <c r="H13" s="2">
+        <v>18392</v>
+      </c>
+      <c r="I13" s="2">
+        <v>17705</v>
+      </c>
+      <c r="J13" s="2">
+        <v>20453</v>
+      </c>
+      <c r="K13" s="2">
+        <v>20674</v>
+      </c>
+      <c r="L13" s="2">
+        <v>21539</v>
+      </c>
+      <c r="M13" s="2">
+        <v>21698</v>
+      </c>
+      <c r="N13" s="2">
+        <v>24188</v>
+      </c>
+      <c r="O13" s="4">
+        <v>23605</v>
+      </c>
+      <c r="P13" s="4">
+        <v>23789</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>23927</v>
+      </c>
+      <c r="R13" s="4">
+        <v>24029</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="2">
+        <v>10506</v>
+      </c>
+      <c r="C14" s="2">
+        <v>11414</v>
+      </c>
+      <c r="D14" s="2">
+        <v>12525</v>
+      </c>
+      <c r="E14" s="2">
+        <v>13283</v>
+      </c>
+      <c r="F14" s="2">
+        <v>14395</v>
+      </c>
+      <c r="G14" s="2">
+        <v>15636</v>
+      </c>
+      <c r="H14" s="2">
+        <v>16045</v>
+      </c>
+      <c r="I14" s="2">
+        <v>15379</v>
+      </c>
+      <c r="J14" s="2">
+        <v>17094</v>
+      </c>
+      <c r="K14" s="2">
+        <v>18986</v>
+      </c>
+      <c r="L14" s="2">
+        <v>19863</v>
+      </c>
+      <c r="M14" s="2">
+        <v>20359</v>
+      </c>
+      <c r="N14" s="2">
+        <v>21552</v>
+      </c>
+      <c r="O14" s="4">
+        <v>20996</v>
+      </c>
+      <c r="P14" s="4">
+        <v>21158</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>21279</v>
+      </c>
+      <c r="R14" s="4">
+        <v>21369</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2">
+        <v>10770</v>
+      </c>
+      <c r="C15" s="2">
+        <v>11579</v>
+      </c>
+      <c r="D15" s="2">
+        <v>12326</v>
+      </c>
+      <c r="E15" s="2">
+        <v>13407</v>
+      </c>
+      <c r="F15" s="2">
+        <v>13735</v>
+      </c>
+      <c r="G15" s="2">
+        <v>15071</v>
+      </c>
+      <c r="H15" s="2">
+        <v>14917</v>
+      </c>
+      <c r="I15" s="2">
+        <v>15990</v>
+      </c>
+      <c r="J15" s="2">
+        <v>17318</v>
+      </c>
+      <c r="K15" s="2">
+        <v>18935</v>
+      </c>
+      <c r="L15" s="2">
+        <v>18217</v>
+      </c>
+      <c r="M15" s="2">
+        <v>18965</v>
+      </c>
+      <c r="N15" s="2">
+        <v>19376</v>
+      </c>
+      <c r="O15" s="4">
+        <v>20069</v>
+      </c>
+      <c r="P15" s="4">
+        <v>20213</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>20320</v>
+      </c>
+      <c r="R15" s="4">
+        <v>20400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="2">
+        <v>11222</v>
+      </c>
+      <c r="C16" s="2">
+        <v>11439</v>
+      </c>
+      <c r="D16" s="2">
+        <v>12150</v>
+      </c>
+      <c r="E16" s="2">
+        <v>13322</v>
+      </c>
+      <c r="F16" s="2">
+        <v>15068</v>
+      </c>
+      <c r="G16" s="2">
+        <v>16103</v>
+      </c>
+      <c r="H16" s="2">
+        <v>15446</v>
+      </c>
+      <c r="I16" s="2">
+        <v>15779</v>
+      </c>
+      <c r="J16" s="2">
+        <v>16495</v>
+      </c>
+      <c r="K16" s="2">
+        <v>19147</v>
+      </c>
+      <c r="L16" s="2">
+        <v>19244</v>
+      </c>
+      <c r="M16" s="2">
+        <v>20062</v>
+      </c>
+      <c r="N16" s="2">
+        <v>21018</v>
+      </c>
+      <c r="O16" s="4">
+        <v>20666</v>
+      </c>
+      <c r="P16" s="4">
+        <v>20819</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>20934</v>
+      </c>
+      <c r="R16" s="4">
+        <v>21019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="2">
+        <v>12122</v>
+      </c>
+      <c r="C17" s="2">
+        <v>13057</v>
+      </c>
+      <c r="D17" s="2">
+        <v>13949</v>
+      </c>
+      <c r="E17" s="2">
+        <v>14734</v>
+      </c>
+      <c r="F17" s="2">
+        <v>16046</v>
+      </c>
+      <c r="G17" s="2">
+        <v>16803</v>
+      </c>
+      <c r="H17" s="2">
+        <v>15816</v>
+      </c>
+      <c r="I17" s="2">
+        <v>17591</v>
+      </c>
+      <c r="J17" s="2">
+        <v>19232</v>
+      </c>
+      <c r="K17" s="2">
+        <v>21090</v>
+      </c>
+      <c r="L17" s="2">
+        <v>21159</v>
+      </c>
+      <c r="M17" s="2">
+        <v>22387</v>
+      </c>
+      <c r="N17" s="2">
+        <v>22324</v>
+      </c>
+      <c r="O17" s="4">
+        <v>22517</v>
+      </c>
+      <c r="P17" s="4">
+        <v>22680</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>22801</v>
+      </c>
+      <c r="R17" s="4">
+        <v>22892</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{308E10F1-8B4F-B945-A167-06E928BEFEC5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660126FC-D371-374B-8EE6-E2A0D2A6094F}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3069,1643 +5514,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ED8B55-971D-A44A-BE5B-A8B57732300D}">
-  <dimension ref="A1:F86"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3">
-        <f>E3/1000</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3">
-        <v>3844</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1990</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1991</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1992</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1993</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="2">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1994</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1995</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="2">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1996</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2">
-        <v>8</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1997</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2">
-        <v>9</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1998</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="2">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1999</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2">
-        <v>11</v>
-      </c>
-      <c r="B16" s="2">
-        <v>2000</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="2">
-        <v>12</v>
-      </c>
-      <c r="B17" s="2">
-        <v>2001</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2">
-        <v>2002</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="2">
-        <v>14</v>
-      </c>
-      <c r="B19" s="2">
-        <v>2003</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="2">
-        <v>15</v>
-      </c>
-      <c r="B20" s="2">
-        <v>2004</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="2">
-        <v>16</v>
-      </c>
-      <c r="B21" s="2">
-        <v>2005</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="2">
-        <v>17</v>
-      </c>
-      <c r="B22" s="2">
-        <v>2006</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="2">
-        <v>18</v>
-      </c>
-      <c r="B23" s="2">
-        <v>2007</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="2">
-        <v>19</v>
-      </c>
-      <c r="B24" s="2">
-        <v>2008</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="2">
-        <v>20</v>
-      </c>
-      <c r="B25" s="2">
-        <v>2009</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="2">
-        <v>21</v>
-      </c>
-      <c r="B26" s="2">
-        <v>2010</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="2">
-        <v>22</v>
-      </c>
-      <c r="B27" s="2">
-        <v>2011</v>
-      </c>
-      <c r="C27" s="3">
-        <v>0</v>
-      </c>
-      <c r="D27" s="3">
-        <v>0</v>
-      </c>
-      <c r="E27" s="3">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="2">
-        <v>23</v>
-      </c>
-      <c r="B28" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C28" s="3">
-        <v>0</v>
-      </c>
-      <c r="D28" s="3">
-        <v>0</v>
-      </c>
-      <c r="E28" s="3">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="2">
-        <v>24</v>
-      </c>
-      <c r="B29" s="2">
-        <v>2013</v>
-      </c>
-      <c r="C29" s="3">
-        <v>0</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0</v>
-      </c>
-      <c r="E29" s="3">
-        <v>0</v>
-      </c>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="2">
-        <v>25</v>
-      </c>
-      <c r="B30" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C30" s="3">
-        <v>0</v>
-      </c>
-      <c r="D30" s="3">
-        <v>0</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="2">
-        <v>26</v>
-      </c>
-      <c r="B31" s="2">
-        <v>2015</v>
-      </c>
-      <c r="C31" s="3">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3">
-        <v>0</v>
-      </c>
-      <c r="E31" s="3">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="2">
-        <v>27</v>
-      </c>
-      <c r="B32" s="2">
-        <v>2016</v>
-      </c>
-      <c r="C32" s="3">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0</v>
-      </c>
-      <c r="E32" s="3">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="2">
-        <v>28</v>
-      </c>
-      <c r="B33" s="2">
-        <v>2017</v>
-      </c>
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-      <c r="D33" s="3">
-        <v>0</v>
-      </c>
-      <c r="E33" s="3">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="2">
-        <v>29</v>
-      </c>
-      <c r="B34" s="2">
-        <v>2018</v>
-      </c>
-      <c r="C34" s="3">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3">
-        <v>0</v>
-      </c>
-      <c r="E34" s="3">
-        <v>0</v>
-      </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="2">
-        <v>30</v>
-      </c>
-      <c r="B35" s="2">
-        <v>2019</v>
-      </c>
-      <c r="C35" s="3">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3">
-        <v>0</v>
-      </c>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="2">
-        <v>31</v>
-      </c>
-      <c r="B36" s="2">
-        <v>2020</v>
-      </c>
-      <c r="C36" s="3">
-        <v>0</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0</v>
-      </c>
-      <c r="E36" s="3">
-        <v>0</v>
-      </c>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="2">
-        <v>32</v>
-      </c>
-      <c r="B37" s="2">
-        <v>2021</v>
-      </c>
-      <c r="C37" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D37" s="3">
-        <v>0</v>
-      </c>
-      <c r="E37" s="3">
-        <v>0</v>
-      </c>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="2">
-        <v>33</v>
-      </c>
-      <c r="B38" s="2">
-        <v>2022</v>
-      </c>
-      <c r="C38" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D38" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E38" s="3">
-        <v>0</v>
-      </c>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="2">
-        <v>34</v>
-      </c>
-      <c r="B39" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C39" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D39" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E39" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="2">
-        <v>35</v>
-      </c>
-      <c r="B40" s="2">
-        <v>2024</v>
-      </c>
-      <c r="C40" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D40" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E40" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="2">
-        <v>36</v>
-      </c>
-      <c r="B41" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C41" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D41" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E41" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="2">
-        <v>37</v>
-      </c>
-      <c r="B42" s="2">
-        <v>2026</v>
-      </c>
-      <c r="C42" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D42" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E42" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="2">
-        <v>38</v>
-      </c>
-      <c r="B43" s="2">
-        <v>2027</v>
-      </c>
-      <c r="C43" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D43" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E43" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="2">
-        <v>39</v>
-      </c>
-      <c r="B44" s="2">
-        <v>2028</v>
-      </c>
-      <c r="C44" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D44" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E44" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="2">
-        <v>40</v>
-      </c>
-      <c r="B45" s="2">
-        <v>2029</v>
-      </c>
-      <c r="C45" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D45" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E45" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="2">
-        <v>41</v>
-      </c>
-      <c r="B46" s="2">
-        <v>2030</v>
-      </c>
-      <c r="C46" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D46" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E46" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="2">
-        <v>42</v>
-      </c>
-      <c r="B47" s="2">
-        <v>2031</v>
-      </c>
-      <c r="C47" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D47" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E47" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="2">
-        <v>43</v>
-      </c>
-      <c r="B48" s="2">
-        <v>2032</v>
-      </c>
-      <c r="C48" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D48" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E48" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="2">
-        <v>44</v>
-      </c>
-      <c r="B49" s="2">
-        <v>2033</v>
-      </c>
-      <c r="C49" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D49" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E49" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="2">
-        <v>45</v>
-      </c>
-      <c r="B50" s="2">
-        <v>2034</v>
-      </c>
-      <c r="C50" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D50" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E50" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="2">
-        <v>46</v>
-      </c>
-      <c r="B51" s="2">
-        <v>2035</v>
-      </c>
-      <c r="C51" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D51" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E51" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="2">
-        <v>47</v>
-      </c>
-      <c r="B52" s="2">
-        <v>2036</v>
-      </c>
-      <c r="C52" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D52" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E52" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="2">
-        <v>48</v>
-      </c>
-      <c r="B53" s="2">
-        <v>2037</v>
-      </c>
-      <c r="C53" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D53" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E53" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="2">
-        <v>49</v>
-      </c>
-      <c r="B54" s="2">
-        <v>2038</v>
-      </c>
-      <c r="C54" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D54" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E54" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="2">
-        <v>50</v>
-      </c>
-      <c r="B55" s="2">
-        <v>2039</v>
-      </c>
-      <c r="C55" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D55" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E55" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="2">
-        <v>51</v>
-      </c>
-      <c r="B56" s="2">
-        <v>2040</v>
-      </c>
-      <c r="C56" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D56" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E56" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="2">
-        <v>52</v>
-      </c>
-      <c r="B57" s="2">
-        <v>2041</v>
-      </c>
-      <c r="C57" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D57" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E57" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="2">
-        <v>53</v>
-      </c>
-      <c r="B58" s="2">
-        <v>2042</v>
-      </c>
-      <c r="C58" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D58" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E58" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="2">
-        <v>54</v>
-      </c>
-      <c r="B59" s="2">
-        <v>2043</v>
-      </c>
-      <c r="C59" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D59" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E59" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="2">
-        <v>55</v>
-      </c>
-      <c r="B60" s="2">
-        <v>2044</v>
-      </c>
-      <c r="C60" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D60" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E60" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="2">
-        <v>56</v>
-      </c>
-      <c r="B61" s="2">
-        <v>2045</v>
-      </c>
-      <c r="C61" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D61" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E61" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="2">
-        <v>57</v>
-      </c>
-      <c r="B62" s="2">
-        <v>2046</v>
-      </c>
-      <c r="C62" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D62" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E62" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="2">
-        <v>58</v>
-      </c>
-      <c r="B63" s="2">
-        <v>2047</v>
-      </c>
-      <c r="C63" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D63" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E63" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="2">
-        <v>59</v>
-      </c>
-      <c r="B64" s="2">
-        <v>2048</v>
-      </c>
-      <c r="C64" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D64" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E64" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="2">
-        <v>60</v>
-      </c>
-      <c r="B65" s="2">
-        <v>2049</v>
-      </c>
-      <c r="C65" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D65" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E65" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="2">
-        <v>61</v>
-      </c>
-      <c r="B66" s="2">
-        <v>2050</v>
-      </c>
-      <c r="C66" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D66" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E66" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="2">
-        <v>62</v>
-      </c>
-      <c r="B67" s="2">
-        <v>2051</v>
-      </c>
-      <c r="C67" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D67" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E67" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="2">
-        <v>63</v>
-      </c>
-      <c r="B68" s="2">
-        <v>2052</v>
-      </c>
-      <c r="C68" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D68" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E68" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="2">
-        <v>64</v>
-      </c>
-      <c r="B69" s="2">
-        <v>2053</v>
-      </c>
-      <c r="C69" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D69" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E69" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="2">
-        <v>65</v>
-      </c>
-      <c r="B70" s="2">
-        <v>2054</v>
-      </c>
-      <c r="C70" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D70" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E70" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="2">
-        <v>66</v>
-      </c>
-      <c r="B71" s="2">
-        <v>2055</v>
-      </c>
-      <c r="C71" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D71" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E71" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="2">
-        <v>67</v>
-      </c>
-      <c r="B72" s="2">
-        <v>2056</v>
-      </c>
-      <c r="C72" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D72" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E72" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="2">
-        <v>68</v>
-      </c>
-      <c r="B73" s="2">
-        <v>2057</v>
-      </c>
-      <c r="C73" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D73" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E73" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="2">
-        <v>69</v>
-      </c>
-      <c r="B74" s="2">
-        <v>2058</v>
-      </c>
-      <c r="C74" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D74" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E74" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="2">
-        <v>70</v>
-      </c>
-      <c r="B75" s="2">
-        <v>2059</v>
-      </c>
-      <c r="C75" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D75" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E75" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="2">
-        <v>71</v>
-      </c>
-      <c r="B76" s="2">
-        <v>2060</v>
-      </c>
-      <c r="C76" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D76" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E76" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="2">
-        <v>72</v>
-      </c>
-      <c r="B77" s="2">
-        <v>2061</v>
-      </c>
-      <c r="C77" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D77" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E77" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="2">
-        <v>73</v>
-      </c>
-      <c r="B78" s="2">
-        <v>2062</v>
-      </c>
-      <c r="C78" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D78" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E78" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="2">
-        <v>74</v>
-      </c>
-      <c r="B79" s="2">
-        <v>2063</v>
-      </c>
-      <c r="C79" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D79" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E79" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="2">
-        <v>75</v>
-      </c>
-      <c r="B80" s="2">
-        <v>2064</v>
-      </c>
-      <c r="C80" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D80" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E80" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="2">
-        <v>76</v>
-      </c>
-      <c r="B81" s="2">
-        <v>2065</v>
-      </c>
-      <c r="C81" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D81" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E81" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="2">
-        <v>77</v>
-      </c>
-      <c r="B82" s="2">
-        <v>2066</v>
-      </c>
-      <c r="C82" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D82" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E82" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="2">
-        <v>78</v>
-      </c>
-      <c r="B83" s="2">
-        <v>2067</v>
-      </c>
-      <c r="C83" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D83" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E83" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
-      <c r="A84" s="2">
-        <v>79</v>
-      </c>
-      <c r="B84" s="2">
-        <v>2068</v>
-      </c>
-      <c r="C84" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D84" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E84" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="2">
-        <v>80</v>
-      </c>
-      <c r="B85" s="2">
-        <v>2069</v>
-      </c>
-      <c r="C85" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D85" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E85" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="2">
-        <v>81</v>
-      </c>
-      <c r="B86" s="2">
-        <v>2070</v>
-      </c>
-      <c r="C86" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="D86" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="E86" s="3">
-        <f>$B$3</f>
-        <v>3.8439999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5064,12 +5878,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1B5589-C105-0C48-A275-3AA9438407BD}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5153,12 +5967,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448ADAEE-828A-6B4D-96D7-60B83E60F26C}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>